<commit_message>
Reorg Main folder, move App stuff to AApp folder
</commit_message>
<xml_diff>
--- a/graphics/layouts/MapToolbox.xlsx
+++ b/graphics/layouts/MapToolbox.xlsx
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AR112"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2:AE28"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9811,6 +9811,7 @@
     <col min="15" max="16" width="2.5703125" customWidth="1"/>
     <col min="17" max="17" width="3.140625" customWidth="1"/>
     <col min="19" max="19" width="3.85546875" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" customWidth="1"/>
     <col min="21" max="21" width="3.85546875" customWidth="1"/>
     <col min="23" max="23" width="3.85546875" customWidth="1"/>
     <col min="25" max="25" width="3.85546875" customWidth="1"/>
@@ -15154,7 +15155,7 @@
   <dimension ref="A2:AS104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AN2" sqref="AN2:AN21"/>
+      <selection activeCell="T2" sqref="T2:T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>